<commit_message>
updating bistline comparison files to include IPM-EPA data
</commit_message>
<xml_diff>
--- a/data-extra/ira_comparison_raw/ira_comparison.xlsx
+++ b/data-extra/ira_comparison_raw/ira_comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrownin\Git Repos\LEEP\data-extra\ira_comparison_raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcole\Documents\LEEP\LEEP\data-extra\ira_comparison_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FFA918-CEB9-4F97-8A6D-8C96E71C6CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E4EA1C-E2AD-45E5-B04D-9491B25C6F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="811" activeTab="1" xr2:uid="{5F00DDB9-0E99-47E0-A966-ACC1987AA917}"/>
+    <workbookView xWindow="705" yWindow="4545" windowWidth="17820" windowHeight="11235" tabRatio="811" firstSheet="3" activeTab="8" xr2:uid="{5F00DDB9-0E99-47E0-A966-ACC1987AA917}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="14" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3051" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3131" uniqueCount="84">
   <si>
     <t>IRA</t>
   </si>
@@ -292,6 +292,12 @@
   </si>
   <si>
     <t>EV Sales Share (%)</t>
+  </si>
+  <si>
+    <t>Reference without IRA</t>
+  </si>
+  <si>
+    <t>IPM-EPA</t>
   </si>
 </sst>
 </file>
@@ -1090,10 +1096,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5BA7B03-7E95-44A8-8E57-7EF481135E5D}">
-  <dimension ref="A1:L145"/>
+  <dimension ref="A1:L147"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView topLeftCell="A139" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J149" sqref="J149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5586,6 +5592,78 @@
         <v>33</v>
       </c>
     </row>
+    <row r="146" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D146" s="3">
+        <v>2400.1</v>
+      </c>
+      <c r="E146" s="3">
+        <v>1551</v>
+      </c>
+      <c r="F146" s="2"/>
+      <c r="G146" s="2">
+        <v>1303.5828442217758</v>
+      </c>
+      <c r="H146" s="2">
+        <v>1247.2876908604831</v>
+      </c>
+      <c r="I146" s="2">
+        <v>1078.2152299012889</v>
+      </c>
+      <c r="J146" s="2">
+        <v>974.78662533547231</v>
+      </c>
+      <c r="K146" s="2">
+        <v>844.16206019677293</v>
+      </c>
+      <c r="L146" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D147" s="3">
+        <v>2400.1</v>
+      </c>
+      <c r="E147" s="3">
+        <v>1551</v>
+      </c>
+      <c r="F147" s="2"/>
+      <c r="G147" s="2">
+        <v>971.71936396552326</v>
+      </c>
+      <c r="H147" s="2">
+        <v>608.29910272708059</v>
+      </c>
+      <c r="I147" s="2">
+        <v>481.36611776682162</v>
+      </c>
+      <c r="J147" s="2">
+        <v>405.7058132501208</v>
+      </c>
+      <c r="K147" s="2">
+        <v>356.71684510032821</v>
+      </c>
+      <c r="L147" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5594,10 +5672,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{690E30FA-4CD4-4165-8253-140D940C5DE0}">
-  <dimension ref="A1:J145"/>
+  <dimension ref="A1:J149"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="J145" sqref="J145:J149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9907,6 +9985,122 @@
         <v>3</v>
       </c>
     </row>
+    <row r="146" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E146" s="3">
+        <v>5.3780147428500582</v>
+      </c>
+      <c r="F146" s="3">
+        <v>5.3780147428500582</v>
+      </c>
+      <c r="G146" s="3">
+        <v>5.3780147428500582</v>
+      </c>
+      <c r="H146" s="3">
+        <v>5.3588452100484147</v>
+      </c>
+      <c r="I146" s="3">
+        <v>5.3588452100484147</v>
+      </c>
+      <c r="J146" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E147" s="3">
+        <v>10.000000489549343</v>
+      </c>
+      <c r="F147" s="3">
+        <v>10.000000489549343</v>
+      </c>
+      <c r="G147" s="3">
+        <v>9.0085890976471568</v>
+      </c>
+      <c r="H147" s="3">
+        <v>5.4817870528002093</v>
+      </c>
+      <c r="I147" s="3">
+        <v>4.4636785382157314</v>
+      </c>
+      <c r="J147" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E148" s="3">
+        <v>88.748458178510205</v>
+      </c>
+      <c r="F148" s="3">
+        <v>100.65357965849033</v>
+      </c>
+      <c r="G148" s="3">
+        <v>73.779766435409613</v>
+      </c>
+      <c r="H148" s="3">
+        <v>5.5265852227694197</v>
+      </c>
+      <c r="I148" s="3">
+        <v>2.991203808895087</v>
+      </c>
+      <c r="J148" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E149" s="3">
+        <v>20.507913569995466</v>
+      </c>
+      <c r="F149" s="3">
+        <v>31.753769509136593</v>
+      </c>
+      <c r="G149" s="3">
+        <v>31.753769509136593</v>
+      </c>
+      <c r="H149" s="3">
+        <v>17.029351904487385</v>
+      </c>
+      <c r="I149" s="3">
+        <v>16.11865922343058</v>
+      </c>
+      <c r="J149" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9916,7 +10110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3BAA39A-0BF4-4085-9680-9F9D9D6B87A8}">
   <dimension ref="A1:J199"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A187" workbookViewId="0">
       <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
@@ -15893,10 +16087,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE0BA1F-1079-4F85-BE53-285F79BAFC0C}">
-  <dimension ref="A1:J109"/>
+  <dimension ref="A1:J121"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A111" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H129" sqref="H129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18911,6 +19105,354 @@
         <v>37</v>
       </c>
     </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E110" s="3">
+        <v>1125.5760699183948</v>
+      </c>
+      <c r="F110" s="3">
+        <v>1168.6392807106861</v>
+      </c>
+      <c r="G110" s="3">
+        <v>1208.1829474458632</v>
+      </c>
+      <c r="H110" s="3">
+        <v>1265.0231814664212</v>
+      </c>
+      <c r="I110" s="3">
+        <v>1316.7229574691614</v>
+      </c>
+      <c r="J110" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E111" s="3">
+        <v>3208.1451654342995</v>
+      </c>
+      <c r="F111" s="3">
+        <v>3321.3472891351075</v>
+      </c>
+      <c r="G111" s="3">
+        <v>3471.7930630963415</v>
+      </c>
+      <c r="H111" s="3">
+        <v>3648.1780877663764</v>
+      </c>
+      <c r="I111" s="3">
+        <v>3866.7500998113555</v>
+      </c>
+      <c r="J111" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E112" s="3">
+        <v>174.52799636670341</v>
+      </c>
+      <c r="F112" s="3">
+        <v>306.32574927068379</v>
+      </c>
+      <c r="G112" s="3">
+        <v>421.72050213235298</v>
+      </c>
+      <c r="H112" s="3">
+        <v>515.21031559513233</v>
+      </c>
+      <c r="I112" s="3">
+        <v>594.45734713116724</v>
+      </c>
+      <c r="J112" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A113" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E113" s="3">
+        <v>0</v>
+      </c>
+      <c r="F113" s="3">
+        <v>0</v>
+      </c>
+      <c r="G113" s="3">
+        <v>0</v>
+      </c>
+      <c r="H113" s="3">
+        <v>0</v>
+      </c>
+      <c r="I113" s="3">
+        <v>0</v>
+      </c>
+      <c r="J113" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A114" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E114" s="3">
+        <v>0</v>
+      </c>
+      <c r="F114" s="3">
+        <v>0</v>
+      </c>
+      <c r="G114" s="3">
+        <v>0</v>
+      </c>
+      <c r="H114" s="3">
+        <v>0</v>
+      </c>
+      <c r="I114" s="3">
+        <v>0</v>
+      </c>
+      <c r="J114" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A115" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E115" s="3">
+        <v>4508.2492317193974</v>
+      </c>
+      <c r="F115" s="3">
+        <v>4796.3123191164768</v>
+      </c>
+      <c r="G115" s="3">
+        <v>5101.6965126745581</v>
+      </c>
+      <c r="H115" s="3">
+        <v>5428.4115848279298</v>
+      </c>
+      <c r="I115" s="3">
+        <v>5777.9304044116834</v>
+      </c>
+      <c r="J115" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E116" s="3">
+        <v>1125.5760699183948</v>
+      </c>
+      <c r="F116" s="3">
+        <v>1168.6392807106861</v>
+      </c>
+      <c r="G116" s="3">
+        <v>1208.1829474458632</v>
+      </c>
+      <c r="H116" s="3">
+        <v>1265.0231814664212</v>
+      </c>
+      <c r="I116" s="3">
+        <v>1316.7229574691614</v>
+      </c>
+      <c r="J116" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E117" s="3">
+        <v>3208.1451654342995</v>
+      </c>
+      <c r="F117" s="3">
+        <v>3321.3472891351075</v>
+      </c>
+      <c r="G117" s="3">
+        <v>3471.7930630963415</v>
+      </c>
+      <c r="H117" s="3">
+        <v>3648.1780877663764</v>
+      </c>
+      <c r="I117" s="3">
+        <v>3866.7500998113555</v>
+      </c>
+      <c r="J117" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E118" s="3">
+        <v>174.52799636670341</v>
+      </c>
+      <c r="F118" s="3">
+        <v>306.32574927068379</v>
+      </c>
+      <c r="G118" s="3">
+        <v>421.72050213235298</v>
+      </c>
+      <c r="H118" s="3">
+        <v>515.21031559513233</v>
+      </c>
+      <c r="I118" s="3">
+        <v>594.45734713116724</v>
+      </c>
+      <c r="J118" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E119" s="3">
+        <v>0</v>
+      </c>
+      <c r="F119" s="3">
+        <v>0</v>
+      </c>
+      <c r="G119" s="3">
+        <v>0</v>
+      </c>
+      <c r="H119" s="3">
+        <v>0</v>
+      </c>
+      <c r="I119" s="3">
+        <v>0</v>
+      </c>
+      <c r="J119" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E120" s="3">
+        <v>0</v>
+      </c>
+      <c r="F120" s="3">
+        <v>0</v>
+      </c>
+      <c r="G120" s="3">
+        <v>0</v>
+      </c>
+      <c r="H120" s="3">
+        <v>0</v>
+      </c>
+      <c r="I120" s="3">
+        <v>0</v>
+      </c>
+      <c r="J120" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E121" s="3">
+        <v>4508.2492317193974</v>
+      </c>
+      <c r="F121" s="3">
+        <v>4796.3123191164768</v>
+      </c>
+      <c r="G121" s="3">
+        <v>5101.6965126745581</v>
+      </c>
+      <c r="H121" s="3">
+        <v>5428.4115848279298</v>
+      </c>
+      <c r="I121" s="3">
+        <v>5777.9304044116834</v>
+      </c>
+      <c r="J121" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18918,10 +19460,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95C08327-8546-4626-8135-5EE1E54ECCE3}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19337,6 +19879,64 @@
         <v>39</v>
       </c>
       <c r="J19" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.48536449106829072</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.42092160324787181</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0.33970812484427471</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0.29303191096310366</v>
+      </c>
+      <c r="I20" s="3">
+        <v>0.22147151555838668</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.3337243671278719</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0.19408027184425583</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0.1473928924446351</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0.10111546375296555</v>
+      </c>
+      <c r="I21" s="3">
+        <v>8.717814044810368E-2</v>
+      </c>
+      <c r="J21" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -21705,7 +22305,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70E3A388-4F05-4E62-A94C-CB27D872236F}">
   <dimension ref="A1:T55"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -24937,11 +25537,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005B8B916ED2FB6A47AFA4E05A3E606BD3" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a94e0fd8b44729910807c0515ebac9ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns5="3d00cabe-74f9-499f-ba26-1e0076cbc6cc" xmlns:ns6="2755580c-7c5f-43cf-bd85-5c868b718937" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6c46c8e9e737c7513e9b5f82e7b81653" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -25362,7 +25957,21 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
@@ -25404,24 +26013,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF3E4C51-E6E8-4BFC-AC40-B34A2F9422A7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA9C6133-5565-4829-8C00-779CE64E6A3A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -25444,7 +26036,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF3E4C51-E6E8-4BFC-AC40-B34A2F9422A7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E1D6D69-9BC6-4995-B2A8-E3FE6BB0C249}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09811017-C1A2-4699-BAC2-9BE21994A32F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -25463,12 +26071,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E1D6D69-9BC6-4995-B2A8-E3FE6BB0C249}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
slight edits to the IPM-EPA data
</commit_message>
<xml_diff>
--- a/data-extra/ira_comparison_raw/ira_comparison.xlsx
+++ b/data-extra/ira_comparison_raw/ira_comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcole\Documents\LEEP\LEEP\data-extra\ira_comparison_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E4EA1C-E2AD-45E5-B04D-9491B25C6F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21B7734-CA6C-47FF-88CD-F357959A0878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="705" yWindow="4545" windowWidth="17820" windowHeight="11235" tabRatio="811" firstSheet="3" activeTab="8" xr2:uid="{5F00DDB9-0E99-47E0-A966-ACC1987AA917}"/>
+    <workbookView xWindow="9105" yWindow="3105" windowWidth="25035" windowHeight="13515" tabRatio="811" activeTab="7" xr2:uid="{5F00DDB9-0E99-47E0-A966-ACC1987AA917}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="14" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3131" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3131" uniqueCount="83">
   <si>
     <t>IRA</t>
   </si>
@@ -292,9 +292,6 @@
   </si>
   <si>
     <t>EV Sales Share (%)</t>
-  </si>
-  <si>
-    <t>Reference without IRA</t>
   </si>
   <si>
     <t>IPM-EPA</t>
@@ -1098,13 +1095,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5BA7B03-7E95-44A8-8E57-7EF481135E5D}">
   <dimension ref="A1:L147"/>
   <sheetViews>
-    <sheetView topLeftCell="A139" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J149" sqref="J149"/>
+    <sheetView topLeftCell="A121" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A146" sqref="A146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="30.42578125" style="3" customWidth="1"/>
@@ -5594,10 +5591,10 @@
     </row>
     <row r="146" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B146" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="B146" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="C146" s="3" t="s">
         <v>46</v>
@@ -5633,7 +5630,7 @@
         <v>0</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C147" s="3" t="s">
         <v>46</v>
@@ -5675,12 +5672,12 @@
   <dimension ref="A1:J149"/>
   <sheetViews>
     <sheetView topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="J145" sqref="J145:J149"/>
+      <selection activeCell="A146" sqref="A146:A147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="9" width="12" bestFit="1" customWidth="1"/>
@@ -9987,10 +9984,10 @@
     </row>
     <row r="146" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B146" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="B146" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="C146" s="3" t="s">
         <v>53</v>
@@ -10016,10 +10013,10 @@
     </row>
     <row r="147" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B147" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="B147" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="C147" s="3" t="s">
         <v>54</v>
@@ -10048,7 +10045,7 @@
         <v>0</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C148" s="3" t="s">
         <v>53</v>
@@ -10077,7 +10074,7 @@
         <v>0</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C149" s="3" t="s">
         <v>54</v>
@@ -16089,13 +16086,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE0BA1F-1079-4F85-BE53-285F79BAFC0C}">
   <dimension ref="A1:J121"/>
   <sheetViews>
-    <sheetView topLeftCell="A111" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H129" sqref="H129"/>
+    <sheetView topLeftCell="A117" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110:A115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="9" width="12" style="3" bestFit="1" customWidth="1"/>
@@ -19107,10 +19104,10 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B110" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="B110" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="C110" s="3" t="s">
         <v>72</v>
@@ -19136,10 +19133,10 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B111" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="C111" s="3" t="s">
         <v>73</v>
@@ -19165,10 +19162,10 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B112" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="B112" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="C112" s="3" t="s">
         <v>74</v>
@@ -19194,10 +19191,10 @@
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B113" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="C113" s="3" t="s">
         <v>75</v>
@@ -19223,10 +19220,10 @@
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B114" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="C114" s="3" t="s">
         <v>76</v>
@@ -19252,10 +19249,10 @@
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B115" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="B115" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="C115" s="3" t="s">
         <v>77</v>
@@ -19284,7 +19281,7 @@
         <v>0</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>72</v>
@@ -19313,7 +19310,7 @@
         <v>0</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C117" s="3" t="s">
         <v>73</v>
@@ -19342,7 +19339,7 @@
         <v>0</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C118" s="3" t="s">
         <v>74</v>
@@ -19371,7 +19368,7 @@
         <v>0</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C119" s="3" t="s">
         <v>75</v>
@@ -19400,7 +19397,7 @@
         <v>0</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C120" s="3" t="s">
         <v>76</v>
@@ -19429,7 +19426,7 @@
         <v>0</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C121" s="3" t="s">
         <v>77</v>
@@ -19463,12 +19460,12 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="3" bestFit="1" customWidth="1"/>
@@ -19884,10 +19881,10 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>39</v>
@@ -19916,7 +19913,7 @@
         <v>0</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>39</v>
@@ -20806,7 +20803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5018F82-05F8-4226-B359-1D0FB4A3757E}">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -22305,7 +22302,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70E3A388-4F05-4E62-A94C-CB27D872236F}">
   <dimension ref="A1:T55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -25537,6 +25534,62 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d00cabe-74f9-499f-ba26-1e0076cbc6cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j747ac98061d40f0aa7bd47e1db5675d>
+    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
+    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2023-01-24T15:33:11+00:00</Document_x0020_Creation_x0020_Date>
+    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
+    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Creator>
+    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </EPA_x0020_Contributor>
+    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005B8B916ED2FB6A47AFA4E05A3E606BD3" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a94e0fd8b44729910807c0515ebac9ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns5="3d00cabe-74f9-499f-ba26-1e0076cbc6cc" xmlns:ns6="2755580c-7c5f-43cf-bd85-5c868b718937" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6c46c8e9e737c7513e9b5f82e7b81653" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -25957,63 +26010,44 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09811017-C1A2-4699-BAC2-9BE21994A32F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2755580c-7c5f-43cf-bd85-5c868b718937"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="3d00cabe-74f9-499f-ba26-1e0076cbc6cc"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E1D6D69-9BC6-4995-B2A8-E3FE6BB0C249}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d00cabe-74f9-499f-ba26-1e0076cbc6cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j747ac98061d40f0aa7bd47e1db5675d>
-    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
-    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2023-01-24T15:33:11+00:00</Document_x0020_Creation_x0020_Date>
-    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
-    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Creator>
-    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </EPA_x0020_Contributor>
-    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF3E4C51-E6E8-4BFC-AC40-B34A2F9422A7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA9C6133-5565-4829-8C00-779CE64E6A3A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26034,41 +26068,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF3E4C51-E6E8-4BFC-AC40-B34A2F9422A7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E1D6D69-9BC6-4995-B2A8-E3FE6BB0C249}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09811017-C1A2-4699-BAC2-9BE21994A32F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2755580c-7c5f-43cf-bd85-5c868b718937"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-    <ds:schemaRef ds:uri="3d00cabe-74f9-499f-ba26-1e0076cbc6cc"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
data issues fixed maybe
</commit_message>
<xml_diff>
--- a/data-extra/ira_comparison_raw/ira_comparison.xlsx
+++ b/data-extra/ira_comparison_raw/ira_comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrownin\GitHub\LEEP\data-extra\ira_comparison_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E76606-4100-4D38-A2FA-9F5F1AFA9A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C4EC21-6CC1-478A-814B-E52D7A3AE105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="828" activeTab="2" xr2:uid="{5F00DDB9-0E99-47E0-A966-ACC1987AA917}"/>
+    <workbookView xWindow="120" yWindow="2340" windowWidth="28680" windowHeight="11250" tabRatio="828" activeTab="3" xr2:uid="{5F00DDB9-0E99-47E0-A966-ACC1987AA917}"/>
   </bookViews>
   <sheets>
     <sheet name="generation" sheetId="16" r:id="rId1"/>
@@ -420,13 +420,7 @@
     <t>Capacity Additions|Electricity|Solar</t>
   </si>
   <si>
-    <t>Capacity Additions|Electricity|Storage</t>
-  </si>
-  <si>
     <t>Capacity Additions|Electricity|Gas|w/ CCS</t>
-  </si>
-  <si>
-    <t>Capacity Retirements|Electricity|Gas</t>
   </si>
   <si>
     <t>Capacity Retirements|Electricity|Nuclear</t>
@@ -441,13 +435,7 @@
     <t>Capacity Retirements|Electricity|Hydro</t>
   </si>
   <si>
-    <t>Capacity Retirements|Electricity|Coal</t>
-  </si>
-  <si>
     <t>Capacity Retirements|Electricity|Solar</t>
-  </si>
-  <si>
-    <t>Capacity Retirements|Electricity|Storage</t>
   </si>
   <si>
     <t>Capacity Additions|Electricity|Gas|w/o CCS|Average 2021-2035</t>
@@ -526,6 +514,18 @@
   </si>
   <si>
     <t>Secondary Energy|Electricity|Other2</t>
+  </si>
+  <si>
+    <t>Capacity Additions|Electricity|Storage Capacity</t>
+  </si>
+  <si>
+    <t>Capacity Retirements|Electricity|Gas|w/o CCS</t>
+  </si>
+  <si>
+    <t>Capacity Retirements|Electricity|Coal|w/o CCS</t>
+  </si>
+  <si>
+    <t>Capacity Retirements|Electricity|Storage Capacity</t>
   </si>
 </sst>
 </file>
@@ -996,10 +996,10 @@
         <v>32</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>84</v>
@@ -1008,7 +1008,7 @@
         <v>85</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>86</v>
@@ -1017,22 +1017,22 @@
         <v>87</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>89</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>90</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>92</v>
@@ -10710,7 +10710,7 @@
   <dimension ref="A1:T55"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10752,7 +10752,7 @@
         <v>96</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>97</v>
@@ -10776,7 +10776,7 @@
         <v>103</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>104</v>
@@ -10785,13 +10785,13 @@
         <v>105</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>106</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="T1" s="3" t="s">
         <v>107</v>
@@ -14154,8 +14154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99E64FD3-40DF-49DE-8E41-9A8578586801}">
   <dimension ref="A1:P73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14213,10 +14213,10 @@
         <v>85</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N1" s="12" t="s">
         <v>91</v>
@@ -17838,8 +17838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48EFD0DC-091E-497D-A6DB-8615CC46A695}">
   <dimension ref="A1:BY24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17847,7 +17847,7 @@
     <col min="1" max="1" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41" style="3" customWidth="1"/>
+    <col min="4" max="4" width="46.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="23" width="7" bestFit="1" customWidth="1"/>
     <col min="24" max="29" width="8" bestFit="1" customWidth="1"/>
     <col min="30" max="31" width="7" bestFit="1" customWidth="1"/>
@@ -19559,7 +19559,7 @@
         <v>113</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>121</v>
+        <v>153</v>
       </c>
       <c r="Y9" s="3">
         <v>2E-3</v>
@@ -19627,7 +19627,7 @@
         <v>113</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:77" x14ac:dyDescent="0.25">
@@ -19641,7 +19641,7 @@
         <v>113</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>123</v>
+        <v>154</v>
       </c>
       <c r="BE11">
         <v>-2.9714999999999998</v>
@@ -19718,7 +19718,7 @@
         <v>113</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="BP12">
         <v>-3.5760000000000001</v>
@@ -19756,7 +19756,7 @@
         <v>113</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="BE13">
         <v>-0.82869999999999999</v>
@@ -19833,7 +19833,7 @@
         <v>113</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="BF14">
         <v>-6.8999999999999999E-3</v>
@@ -19904,7 +19904,7 @@
         <v>113</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="BE15">
         <v>-1.4800000000000001E-2</v>
@@ -19978,7 +19978,7 @@
         <v>113</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>128</v>
+        <v>155</v>
       </c>
       <c r="BE16">
         <v>-1.0562</v>
@@ -20055,7 +20055,7 @@
         <v>113</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="BN17">
         <v>-3.5000000000000001E-3</v>
@@ -20093,7 +20093,7 @@
         <v>113</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="BP18">
         <v>-2.4E-2</v>
@@ -20213,7 +20213,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -20251,7 +20251,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -20289,7 +20289,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>0</v>
@@ -20327,7 +20327,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>0</v>
@@ -20365,7 +20365,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>0</v>
@@ -20403,7 +20403,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>0</v>
@@ -20441,7 +20441,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>0</v>
@@ -20479,7 +20479,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>0</v>
@@ -20517,7 +20517,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>0</v>
@@ -20555,7 +20555,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>0</v>
@@ -20593,7 +20593,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>0</v>
@@ -20628,7 +20628,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>0</v>
@@ -20663,7 +20663,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>0</v>
@@ -20698,7 +20698,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>52</v>
@@ -20736,7 +20736,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>52</v>
@@ -20774,7 +20774,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>52</v>
@@ -20812,7 +20812,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>52</v>
@@ -20850,7 +20850,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>52</v>
@@ -20888,7 +20888,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>52</v>
@@ -20926,7 +20926,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>52</v>
@@ -20964,7 +20964,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>52</v>
@@ -21002,7 +21002,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>52</v>
@@ -21040,7 +21040,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>52</v>
@@ -21078,7 +21078,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>52</v>
@@ -21113,7 +21113,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>52</v>
@@ -21148,7 +21148,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>52</v>
@@ -39559,6 +39559,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005B8B916ED2FB6A47AFA4E05A3E606BD3" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a94e0fd8b44729910807c0515ebac9ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns5="3d00cabe-74f9-499f-ba26-1e0076cbc6cc" xmlns:ns6="2755580c-7c5f-43cf-bd85-5c868b718937" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6c46c8e9e737c7513e9b5f82e7b81653" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -39979,21 +39984,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
@@ -40035,7 +40026,24 @@
 </p:properties>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF3E4C51-E6E8-4BFC-AC40-B34A2F9422A7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA9C6133-5565-4829-8C00-779CE64E6A3A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -40058,23 +40066,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF3E4C51-E6E8-4BFC-AC40-B34A2F9422A7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E1D6D69-9BC6-4995-B2A8-E3FE6BB0C249}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09811017-C1A2-4699-BAC2-9BE21994A32F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -40093,4 +40085,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E1D6D69-9BC6-4995-B2A8-E3FE6BB0C249}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>